<commit_message>
correction Exemple après test et ajout information procédure
</commit_message>
<xml_diff>
--- a/Documentation/options.xlsx
+++ b/Documentation/options.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Nom de l'option</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>-m</t>
+  </si>
+  <si>
+    <t>image seule</t>
+  </si>
+  <si>
+    <t>permet d'ajouter la même vignette unique dans tous les lots</t>
+  </si>
+  <si>
+    <t>-is</t>
+  </si>
+  <si>
+    <t>Ajouter l'image à dispatcher dans chaque lot au niveau du programme prepalots.py et la renommer vignette.jpg</t>
   </si>
 </sst>
 </file>
@@ -432,21 +444,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="46.7265625" customWidth="1"/>
-    <col min="3" max="3" width="44.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -474,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -488,7 +500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -502,59 +514,73 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout option date dans doc
</commit_message>
<xml_diff>
--- a/Documentation/options.xlsx
+++ b/Documentation/options.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Nom de l'option</t>
   </si>
@@ -39,9 +39,6 @@
     <t>permet de diviser les items en thématique/catégories</t>
   </si>
   <si>
-    <t>Fonctionne en association avec les commandes pdf ou images. Ne fonctionne pas seul.</t>
-  </si>
-  <si>
     <t>PDF</t>
   </si>
   <si>
@@ -118,6 +115,21 @@
   </si>
   <si>
     <t>Ajouter l'image à dispatcher dans chaque lot au niveau du programme prepalots.py et la renommer vignette.jpg</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>permet de diviser les items dans des dossiers date</t>
+  </si>
+  <si>
+    <t>-d</t>
+  </si>
+  <si>
+    <t>Utilise les informations de la colonne Thématique</t>
+  </si>
+  <si>
+    <t>Utilise les informations de la colonne Date de production</t>
   </si>
 </sst>
 </file>
@@ -444,21 +456,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.7265625" customWidth="1"/>
+    <col min="3" max="3" width="44.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,7 +484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -480,108 +492,122 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>